<commit_message>
Upload all data and code for L&O Submission 5/16/24 attempt 2 at 13:42
</commit_message>
<xml_diff>
--- a/Data/Sargassum_recalcitrance.xlsx
+++ b/Data/Sargassum_recalcitrance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chanceenglish/Desktop/Lab Shiz/BIOSSCOPE/SDOM/BIOS-SCOPE-SargassumDOM/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FA2AFE-1470-F540-94C4-3C2F3F9807EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356B94FE-73F3-794A-9C40-89A7E3784F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A229C97A-981F-DE4A-9790-434D5BD8C607}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{A229C97A-981F-DE4A-9790-434D5BD8C607}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1155,7 +1155,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1251,17 +1251,17 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="J2" s="2">
-        <v>0.25286818950000001</v>
+        <v>0.6</v>
       </c>
       <c r="K2" s="1">
         <v>25.337658344208606</v>
       </c>
       <c r="L2" s="2">
         <f>(I2/100)*K2</f>
-        <v>0.96283101707992702</v>
+        <v>0.8868180420473013</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" ref="M2:M9" si="0">(F2/100)*K2</f>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="P2" s="2">
         <f t="shared" ref="P2:P9" si="2">SUM(L2+O2)</f>
-        <v>2.5084281760766522</v>
+        <v>2.4324152010440265</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -1309,7 +1309,7 @@
         <v>37.200000000000003</v>
       </c>
       <c r="J3" s="2">
-        <v>0.71879976599999984</v>
+        <v>0.1</v>
       </c>
       <c r="K3" s="1">
         <v>13.945497386258197</v>
@@ -1361,17 +1361,17 @@
         <v>1.2322341957460639E-3</v>
       </c>
       <c r="I4">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="J4" s="2">
-        <v>0.29271602200000002</v>
+        <v>0.6</v>
       </c>
       <c r="K4" s="1">
         <v>18.221982658528525</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" si="4"/>
-        <v>0.69243534102408388</v>
+        <v>0.63776939304849845</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" si="0"/>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="P4" s="2">
         <f t="shared" si="2"/>
-        <v>1.803976283194324</v>
+        <v>1.7493103352187385</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -1419,7 +1419,7 @@
         <v>37.200000000000003</v>
       </c>
       <c r="J5" s="2">
-        <v>0.98819357050000023</v>
+        <v>0.1</v>
       </c>
       <c r="K5" s="1">
         <v>9.1028268356075515</v>
@@ -1474,7 +1474,7 @@
         <v>12</v>
       </c>
       <c r="J6" s="2">
-        <v>0.57462419499999995</v>
+        <v>0.1</v>
       </c>
       <c r="K6" s="1">
         <v>4.4399791035919094</v>
@@ -1529,7 +1529,7 @@
         <v>27.4</v>
       </c>
       <c r="J7" s="2">
-        <v>0.91292394799999987</v>
+        <v>0.1</v>
       </c>
       <c r="K7" s="1">
         <v>4.9013232341185073</v>
@@ -1584,7 +1584,7 @@
         <v>12</v>
       </c>
       <c r="J8" s="2">
-        <v>0.67547975449999997</v>
+        <v>0.1</v>
       </c>
       <c r="K8" s="1">
         <v>2.9121519335617236</v>
@@ -1639,7 +1639,7 @@
         <v>27.4</v>
       </c>
       <c r="J9" s="2">
-        <v>1.054328377</v>
+        <v>0.1</v>
       </c>
       <c r="K9" s="1">
         <v>6.2923591838367088</v>

</xml_diff>